<commit_message>
Structure Created, seperate Notebooks
</commit_message>
<xml_diff>
--- a/data/Observed_discharge_upto_basantpur_2000_2014.xlsx
+++ b/data/Observed_discharge_upto_basantpur_2000_2014.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rajan_Prasad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LSTM-Flood-Forecasting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2743BC67-048C-4E29-A939-AD9902EE5195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7368"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Andhiyarkhore</t>
   </si>
@@ -46,11 +47,14 @@
   <si>
     <t>Simga</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,12 +381,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1831"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -390,7 +392,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>